<commit_message>
add generate unique tags machinery
</commit_message>
<xml_diff>
--- a/backend/web/templates/machinery_template.xlsx
+++ b/backend/web/templates/machinery_template.xlsx
@@ -1,21 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A665AD-81E8-47E3-939A-9078C2FBDB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="345" yWindow="2205" windowWidth="27630" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Compañía*</t>
   </si>
@@ -90,28 +108,23 @@
   </si>
   <si>
     <t>-29.9574,-71.3089</t>
+  </si>
+  <si>
+    <t>Unique Tag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -150,16 +163,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F989AD9B-3609-4D7A-8DB9-3BE997D3FEC0}" name="DataTblUnique" displayName="DataTblUnique" ref="A1:H2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:H2" xr:uid="{F989AD9B-3609-4D7A-8DB9-3BE997D3FEC0}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{0BE369B8-4517-43C6-85F3-9EA336F6A6CA}" name="Compañía*" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1E4870ED-6261-42EC-9AC2-B6826899DE5A}" name="Proceso Minero*" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{A52BB7A7-B34E-4FAB-AE72-EB1B39FD845C}" name="Familia Equipos* (SEMI/MOVIL/FIJO)" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{D93D7125-4304-43AC-B71E-448654D085B7}" name="Área*" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{6B87FF46-10AF-4B2D-9C34-93AC3AB554AB}" name="Planta/Flota*" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{70F06E5E-CD35-4938-9FA7-4037404BCFE5}" name="Tipo de Equipo*" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{5565C562-8FCA-4736-823E-3F0DBE046C58}" name="Tag/Código*" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{6F6EB56A-239E-425A-A54A-ADC129DEC811}" name="Unique Tag">
+      <calculatedColumnFormula>IF(
+  COUNTA(
+    DataTblUnique[[#This Row],[Tag/Código*]],
+    DataTblUnique[[#This Row],[Tipo de Equipo*]],
+    DataTblUnique[[#This Row],[Planta/Flota*]],
+    DataTblUnique[[#This Row],[Área*]],
+    DataTblUnique[[#This Row],[Familia Equipos* (SEMI/MOVIL/FIJO)]],
+    DataTblUnique[[#This Row],[Proceso Minero*]],
+    DataTblUnique[[#This Row],[Compañía*]]
+  )=0,
+  "",
+  SUBSTITUTE(
+    DataTblUnique[[#This Row],[Tag/Código*]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Tipo de Equipo*]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Planta/Flota*]]   &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Área*]]           &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Familia Equipos* (SEMI/MOVIL/FIJO)]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Proceso Minero*]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Compañía*]],
+    " ",
+    "_"
+  )
+)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,35 +598,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2:N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="41.133" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="37.705" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="25.851" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="74.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,28 +646,31 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -542,31 +692,58 @@
       <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="str">
+        <f>IF(
+  COUNTA(
+    DataTblUnique[[#This Row],[Tag/Código*]],
+    DataTblUnique[[#This Row],[Tipo de Equipo*]],
+    DataTblUnique[[#This Row],[Planta/Flota*]],
+    DataTblUnique[[#This Row],[Área*]],
+    DataTblUnique[[#This Row],[Familia Equipos* (SEMI/MOVIL/FIJO)]],
+    DataTblUnique[[#This Row],[Proceso Minero*]],
+    DataTblUnique[[#This Row],[Compañía*]]
+  )=0,
+  "",
+  SUBSTITUTE(
+    DataTblUnique[[#This Row],[Tag/Código*]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Tipo de Equipo*]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Planta/Flota*]]   &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Área*]]           &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Familia Equipos* (SEMI/MOVIL/FIJO)]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Proceso Minero*]] &amp; "-" &amp;
+    DataTblUnique[[#This Row],[Compañía*]],
+    " ",
+    "_"
+  )
+)</f>
+        <v>CAEX-001-CAEX-CAEX-KMTSU-TRANSPORTE_MINA-MOBILE-EXTRACCIÓN-EL_TOFO</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>800000</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>